<commit_message>
Found a additional dataset and cleaned some of the data for future use
I have tidied a huge portion of the data currently i want to use the first two datasets in the code separately and the last two as a unit with another additional dataset.

i am also thinking of using one of the first data sets with just the 2018 date to show correlation of it with the third data set in the code.
</commit_message>
<xml_diff>
--- a/Datasets/Mental Illness Survey 1.xlsx
+++ b/Datasets/Mental Illness Survey 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\Data_All_190402\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\6006\Course work\9789180-SI-s1\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BD4850-5EBE-4310-8851-CC6B35B8CA58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089F6DC7-7452-4384-956E-4DB477B33745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1646,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>